<commit_message>
added project10 and other fixes
</commit_message>
<xml_diff>
--- a/Project9/NH3/reactants/NH2/nh2_opt.xlsx
+++ b/Project9/NH3/reactants/NH2/nh2_opt.xlsx
@@ -459,13 +459,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>13.436</v>
+        <v>13.693</v>
       </c>
       <c r="C2" t="n">
-        <v>6.036</v>
+        <v>6.032</v>
       </c>
       <c r="D2" t="n">
-        <v>46.543</v>
+        <v>46.524</v>
       </c>
     </row>
     <row r="3">
@@ -513,7 +513,7 @@
         <v>2.981</v>
       </c>
       <c r="D5" t="n">
-        <v>10.895</v>
+        <v>10.876</v>
       </c>
     </row>
     <row r="6">
@@ -523,13 +523,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11.659</v>
+        <v>11.915</v>
       </c>
       <c r="C6" t="n">
-        <v>0.075</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D6" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
     </row>
   </sheetData>
@@ -607,13 +607,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>53.6496</v>
+        <v>53.1545</v>
       </c>
       <c r="C4" t="n">
-        <v>1.729566</v>
+        <v>1.72554</v>
       </c>
       <c r="D4" t="n">
-        <v>3.982474</v>
+        <v>3.973203</v>
       </c>
     </row>
     <row r="5">
@@ -623,13 +623,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.773845</v>
+        <v>0.497165</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.111346</v>
+        <v>-0.303499</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.256384</v>
+        <v>-0.698833</v>
       </c>
     </row>
     <row r="6">
@@ -639,13 +639,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>270585000</v>
+        <v>268073000</v>
       </c>
       <c r="C6" t="n">
-        <v>8.432302999999999</v>
+        <v>8.428253</v>
       </c>
       <c r="D6" t="n">
-        <v>19.416096</v>
+        <v>19.406769</v>
       </c>
     </row>
     <row r="7">
@@ -655,13 +655,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.86194e-09</v>
+        <v>1.85581e-09</v>
       </c>
       <c r="C7" t="n">
-        <v>-8.543340000000001</v>
+        <v>-8.731467</v>
       </c>
       <c r="D7" t="n">
-        <v>-19.671766</v>
+        <v>-20.104945</v>
       </c>
     </row>
     <row r="8">
@@ -671,13 +671,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.00071</v>
+        <v>1.00066</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00031</v>
+        <v>0.000285</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000714</v>
+        <v>0.000657</v>
       </c>
     </row>
   </sheetData>
@@ -708,22 +708,22 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-55.8601196119</v>
+        <v>-55.8846012853</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>-55.8603463303</v>
+        <v>-55.8854240101</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-55.86036107</v>
+        <v>-55.8854468845</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>-55.86036107</v>
+        <v>-55.8854468845</v>
       </c>
     </row>
     <row r="7">
@@ -759,13 +759,13 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2.42273</v>
+        <v>2.56951</v>
       </c>
       <c r="B14" t="n">
-        <v>4.99767</v>
+        <v>4.71312</v>
       </c>
       <c r="C14" t="n">
-        <v>7.4204</v>
+        <v>7.28263</v>
       </c>
     </row>
     <row r="16">
@@ -801,13 +801,13 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>35.75049</v>
+        <v>33.70824</v>
       </c>
       <c r="B23" t="n">
-        <v>17.33084</v>
+        <v>18.37718</v>
       </c>
       <c r="C23" t="n">
-        <v>11.67239</v>
+        <v>11.8932</v>
       </c>
     </row>
     <row r="25">
@@ -819,13 +819,13 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>744.92024</v>
+        <v>702.36667</v>
       </c>
       <c r="B26" t="n">
-        <v>361.11659</v>
+        <v>382.91883</v>
       </c>
       <c r="C26" t="n">
-        <v>243.21347</v>
+        <v>247.81445</v>
       </c>
     </row>
     <row r="28">
@@ -837,7 +837,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>48767.3</v>
+        <v>49841</v>
       </c>
     </row>
     <row r="31">
@@ -849,7 +849,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>11.65566</v>
+        <v>11.91228</v>
       </c>
     </row>
     <row r="34">
@@ -861,13 +861,13 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2160.33</v>
+        <v>2184.78</v>
       </c>
       <c r="B35" t="n">
-        <v>4693.27</v>
+        <v>4828.4</v>
       </c>
       <c r="C35" t="n">
-        <v>4877.1</v>
+        <v>4975.79</v>
       </c>
     </row>
     <row r="37">
@@ -879,7 +879,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.018574</v>
+        <v>0.018983</v>
       </c>
     </row>
     <row r="40">
@@ -891,7 +891,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.021412</v>
+        <v>0.021821</v>
       </c>
     </row>
     <row r="43">
@@ -903,7 +903,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.022356</v>
+        <v>0.022765</v>
       </c>
     </row>
     <row r="46">
@@ -915,7 +915,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.000242</v>
+        <v>0.00066</v>
       </c>
     </row>
     <row r="49">
@@ -927,13 +927,13 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1501.5064</v>
+        <v>1518.503</v>
       </c>
       <c r="B50" t="n">
-        <v>3261.9923</v>
+        <v>3355.9093</v>
       </c>
       <c r="C50" t="n">
-        <v>3389.7557</v>
+        <v>3458.3495</v>
       </c>
     </row>
     <row r="52">
@@ -945,13 +945,13 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1.0994</v>
+        <v>1.0917</v>
       </c>
       <c r="B53" t="n">
-        <v>1.0428</v>
+        <v>1.0498</v>
       </c>
       <c r="C53" t="n">
-        <v>1.0939</v>
+        <v>1.0902</v>
       </c>
     </row>
     <row r="55">
@@ -963,13 +963,13 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1.4603</v>
+        <v>1.4831</v>
       </c>
       <c r="B56" t="n">
-        <v>6.5373</v>
+        <v>6.9659</v>
       </c>
       <c r="C56" t="n">
-        <v>7.4054</v>
+        <v>7.6825</v>
       </c>
     </row>
     <row r="58">
@@ -981,13 +981,13 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>19.2888</v>
+        <v>23.3897</v>
       </c>
       <c r="B59" t="n">
-        <v>47.5932</v>
+        <v>16.2446</v>
       </c>
       <c r="C59" t="n">
-        <v>6.1281</v>
+        <v>2.4019</v>
       </c>
     </row>
   </sheetData>

</xml_diff>